<commit_message>
drop duplicates and round columns
</commit_message>
<xml_diff>
--- a/распереление дат тестирование/graphic-test.xlsx
+++ b/распереление дат тестирование/graphic-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mi\jupyterProjects\tom's work\распереление дат тестирование\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriali/JupyterProjects/tom's work/распереление дат тестирование/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC047FB8-C97A-4944-8569-DF6FF2FB7E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74791799-E08D-E34D-818C-D243FA915D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{1FBC3244-FC2C-49DA-9EE2-02C136ABAD5A}"/>
+    <workbookView xWindow="5140" yWindow="2000" windowWidth="24260" windowHeight="13140" xr2:uid="{1FBC3244-FC2C-49DA-9EE2-02C136ABAD5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Пункт отгрузки</t>
   </si>
@@ -157,11 +157,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -487,83 +485,100 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="A3:D6"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>1779443</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>44723</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1779443</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44724</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1779443</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44725</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>